<commit_message>
fixed data entry error on row 941
</commit_message>
<xml_diff>
--- a/data/raw/USFWS_bull_trout_SSA_data_ID.xlsx
+++ b/data/raw/USFWS_bull_trout_SSA_data_ID.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scheuerl/Documents/GitHub/bulltrout/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scheuerl/Documents/GitHub/bulltrout/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B96C150-5F71-4D4A-9BEA-ACB50F56292E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358BB07F-A931-DB4C-95A4-D3971AD2A7C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="460" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -904,7 +904,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BB1300"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A925" workbookViewId="0">
+      <selection activeCell="A942" sqref="A942"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -25400,7 +25402,7 @@
     </row>
     <row r="941" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A941" s="12">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B941" s="12" t="s">
         <v>44</v>
@@ -25409,7 +25411,7 @@
         <v>62</v>
       </c>
       <c r="D941" s="12" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="E941" s="12" t="s">
         <v>7</v>
@@ -35314,12 +35316,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -35520,15 +35519,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFAABD42-B977-47B6-983A-D015976BBDFC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{407EB793-7EF8-47E0-9BDA-5F3E759227C3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="61093040-1240-489f-8ca6-d5903aeb7a38"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="dbfd3e1b-9f3f-4f6f-b75c-e8eed26c7c7e"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -35553,18 +35564,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{407EB793-7EF8-47E0-9BDA-5F3E759227C3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFAABD42-B977-47B6-983A-D015976BBDFC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="61093040-1240-489f-8ca6-d5903aeb7a38"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="dbfd3e1b-9f3f-4f6f-b75c-e8eed26c7c7e"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>